<commit_message>
Proveedores y Libros de Facturas
Se han creado pantalla y ficheros para proveedores y se han creado dos reports
</commit_message>
<xml_diff>
--- a/PRÉSTAMOS/AEAT.xlsx
+++ b/PRÉSTAMOS/AEAT.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
   <si>
     <t>IVA1T</t>
   </si>
@@ -408,18 +408,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="A2" sqref="A2:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="6.88671875" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -445,72 +445,75 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>42799</v>
+        <v>42921</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="1"/>
       <c r="E2" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="2">
         <v>425.33</v>
       </c>
-      <c r="G2">
-        <v>2.84</v>
+      <c r="G2" s="2">
+        <v>6.82</v>
       </c>
       <c r="H2" s="2">
-        <f>F2+G2</f>
-        <v>428.16999999999996</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+        <v>432.15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>42830</v>
+        <v>42936</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="1"/>
       <c r="E3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="2">
-        <v>425.33</v>
-      </c>
-      <c r="G3">
-        <v>4.1500000000000004</v>
+        <v>348.53</v>
+      </c>
+      <c r="G3" s="2">
+        <v>3.26</v>
       </c>
       <c r="H3" s="2">
-        <f t="shared" ref="H3:H4" si="0">F3+G3</f>
-        <v>429.47999999999996</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+        <v>351.79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>42860</v>
+        <v>42954</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="1"/>
       <c r="E4" t="s">
         <v>0</v>
       </c>
       <c r="F4" s="2">
         <v>425.33</v>
       </c>
-      <c r="G4">
-        <v>5.51</v>
+      <c r="G4" s="2">
+        <v>8.17</v>
       </c>
       <c r="H4" s="2">
-        <f t="shared" si="0"/>
-        <v>430.84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>433.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>42906</v>
+        <v>42968</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
@@ -524,15 +527,15 @@
         <v>348.53</v>
       </c>
       <c r="G5" s="2">
-        <v>2.1800000000000002</v>
+        <v>4.37</v>
       </c>
       <c r="H5" s="2">
-        <v>350.71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+        <v>352.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>42921</v>
+        <v>42983</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>9</v>
@@ -543,18 +546,18 @@
         <v>0</v>
       </c>
       <c r="F6" s="2">
-        <v>425.33</v>
+        <v>425.35</v>
       </c>
       <c r="G6" s="2">
-        <v>6.82</v>
+        <v>9.5299999999999994</v>
       </c>
       <c r="H6" s="2">
-        <v>432.15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>434.88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>42936</v>
+        <v>42998</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>9</v>
@@ -568,15 +571,15 @@
         <v>348.53</v>
       </c>
       <c r="G7" s="2">
-        <v>3.26</v>
+        <v>5.48</v>
       </c>
       <c r="H7" s="2">
-        <v>351.79</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>354.01</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>42954</v>
+        <v>43028</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
@@ -584,21 +587,21 @@
       <c r="C8" s="3"/>
       <c r="D8" s="1"/>
       <c r="E8" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="2">
-        <v>425.33</v>
+        <v>348.53</v>
       </c>
       <c r="G8" s="2">
-        <v>8.17</v>
+        <v>6.55</v>
       </c>
       <c r="H8" s="2">
-        <v>433.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <v>355.08</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>42968</v>
+        <v>43059</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>9</v>
@@ -609,106 +612,18 @@
         <v>1</v>
       </c>
       <c r="F9" s="2">
-        <v>348.53</v>
+        <v>348.56</v>
       </c>
       <c r="G9" s="2">
-        <v>4.37</v>
+        <v>7.66</v>
       </c>
       <c r="H9" s="2">
-        <v>352.9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>42983</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="1"/>
-      <c r="E10" t="s">
-        <v>0</v>
-      </c>
-      <c r="F10" s="2">
-        <v>425.35</v>
-      </c>
-      <c r="G10" s="2">
-        <v>9.5299999999999994</v>
-      </c>
-      <c r="H10" s="2">
-        <v>434.88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>42998</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="1"/>
-      <c r="E11" t="s">
-        <v>1</v>
-      </c>
-      <c r="F11" s="2">
-        <v>348.53</v>
-      </c>
-      <c r="G11" s="2">
-        <v>5.48</v>
-      </c>
-      <c r="H11" s="2">
-        <v>354.01</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
-        <v>43028</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="1"/>
-      <c r="E12" t="s">
-        <v>1</v>
-      </c>
-      <c r="F12" s="2">
-        <v>348.53</v>
-      </c>
-      <c r="G12" s="2">
-        <v>6.55</v>
-      </c>
-      <c r="H12" s="2">
-        <v>355.08</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <v>43059</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="1"/>
-      <c r="E13" t="s">
-        <v>1</v>
-      </c>
-      <c r="F13" s="2">
-        <v>348.56</v>
-      </c>
-      <c r="G13" s="2">
-        <v>7.66</v>
-      </c>
-      <c r="H13" s="2">
         <v>356.22</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:H13">
-    <sortCondition ref="A5:A13"/>
+  <sortState ref="A2:H9">
+    <sortCondition ref="A4:A9"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>